<commit_message>
tabulacion del json OK. Ahora vamos a por los boxes.
</commit_message>
<xml_diff>
--- a/inventario_reformed.xlsx
+++ b/inventario_reformed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\projects\service_report_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\WebDeveloperCourse\projects\service_report_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08A2AB76-8F60-4CAC-B8C3-3DC29E3E0BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39230E37-ECF6-4F06-85DB-C20C226136AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B71063B-2E92-4D3F-94BA-156C7E6719CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4B71063B-2E92-4D3F-94BA-156C7E6719CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2281,21 +2281,9 @@
     <t>SERIE</t>
   </si>
   <si>
-    <t>REGISTRO SANITARIO</t>
-  </si>
-  <si>
     <t>RIESGO</t>
   </si>
   <si>
-    <t>UBICACIÓN</t>
-  </si>
-  <si>
-    <t>ASIGNADO A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVO FIJO </t>
-  </si>
-  <si>
     <t>ESTADO</t>
   </si>
   <si>
@@ -2441,6 +2429,18 @@
   </si>
   <si>
     <t>Flujometro aire y oxigeno, control de mando codigo azul.</t>
+  </si>
+  <si>
+    <t>REGISTRO_SANITARIO</t>
+  </si>
+  <si>
+    <t>ASIGNADO_A</t>
+  </si>
+  <si>
+    <t>ACTIVO_FIJO</t>
+  </si>
+  <si>
+    <t>UBICACION</t>
   </si>
 </sst>
 </file>
@@ -3044,27 +3044,27 @@
   <dimension ref="A1:L332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="3"/>
+    <col min="4" max="4" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>743</v>
       </c>
@@ -3081,28 +3081,28 @@
         <v>747</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3210,7 +3210,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3857,10 +3857,10 @@
         <v>8</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3895,10 +3895,10 @@
         <v>8</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3933,10 +3933,10 @@
         <v>8</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3971,10 +3971,10 @@
         <v>8</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -4009,10 +4009,10 @@
         <v>8</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -4047,10 +4047,10 @@
         <v>8</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -4085,10 +4085,10 @@
         <v>8</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -4123,10 +4123,10 @@
         <v>8</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -4161,10 +4161,10 @@
         <v>8</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -4199,10 +4199,10 @@
         <v>37</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -4237,10 +4237,10 @@
         <v>37</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -4275,10 +4275,10 @@
         <v>37</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -4313,10 +4313,10 @@
         <v>37</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -4351,10 +4351,10 @@
         <v>37</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -4389,10 +4389,10 @@
         <v>37</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -4427,10 +4427,10 @@
         <v>37</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -4465,10 +4465,10 @@
         <v>37</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4503,10 +4503,10 @@
         <v>37</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4541,10 +4541,10 @@
         <v>37</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="L42" s="10"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="L43" s="10"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="L44" s="10"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="L45" s="10"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="L46" s="10"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="L48" s="10"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="L49" s="10"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="L50" s="10"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4920,7 +4920,7 @@
       </c>
       <c r="L51" s="10"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="L52" s="10"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="L53" s="10"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="L54" s="10"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="L55" s="10"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
       <c r="L56" s="10"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="L57" s="10"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="L58" s="10"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -5192,7 +5192,7 @@
       </c>
       <c r="L59" s="10"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="L60" s="10"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -5260,7 +5260,7 @@
       </c>
       <c r="L61" s="10"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="L62" s="10"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -5328,7 +5328,7 @@
       </c>
       <c r="L63" s="10"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="L64" s="10"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -5396,7 +5396,7 @@
       </c>
       <c r="L65" s="10"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="L66" s="10"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="L67" s="10"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="L68" s="10"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="L69" s="10"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="L70" s="10"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -5600,7 +5600,7 @@
       </c>
       <c r="L71" s="10"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="L72" s="10"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="L73" s="10"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="L74" s="10"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -5736,7 +5736,7 @@
       </c>
       <c r="L75" s="10"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="L76" s="10"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="L77" s="10"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="L78" s="10"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="L79" s="10"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -5906,7 +5906,7 @@
       </c>
       <c r="L80" s="10"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -5940,7 +5940,7 @@
       </c>
       <c r="L81" s="10"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="L82" s="10"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="L83" s="10"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -6042,7 +6042,7 @@
       </c>
       <c r="L84" s="10"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -6074,7 +6074,7 @@
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -6106,7 +6106,7 @@
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -6170,7 +6170,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -6276,7 +6276,7 @@
       </c>
       <c r="L91" s="10"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="L92" s="10"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -6344,7 +6344,7 @@
       </c>
       <c r="L93" s="10"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="L94" s="10"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -6412,7 +6412,7 @@
       </c>
       <c r="L95" s="10"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="L96" s="10"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -6480,7 +6480,7 @@
       </c>
       <c r="L97" s="10"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="L98" s="10"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -6548,7 +6548,7 @@
       </c>
       <c r="L99" s="10"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="L100" s="10"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -6618,7 +6618,7 @@
       </c>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -6761,10 +6761,10 @@
         <v>37</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -6800,7 +6800,7 @@
       </c>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -6836,7 +6836,7 @@
       </c>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -6943,10 +6943,10 @@
         <v>37</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -6982,7 +6982,7 @@
       </c>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -7017,10 +7017,10 @@
         <v>37</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="L113" s="4"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="L114" s="4"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -7127,10 +7127,10 @@
         <v>37</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="L117" s="4"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="L118" s="4"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -7346,7 +7346,7 @@
       </c>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -7382,7 +7382,7 @@
       </c>
       <c r="L122" s="4"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -7418,7 +7418,7 @@
       </c>
       <c r="L123" s="4"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -7490,7 +7490,7 @@
       </c>
       <c r="L125" s="4"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -7558,7 +7558,7 @@
       </c>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -7594,7 +7594,7 @@
       </c>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -7698,7 +7698,7 @@
       </c>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -7731,10 +7731,10 @@
         <v>37</v>
       </c>
       <c r="L132" s="4" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -7767,10 +7767,10 @@
         <v>37</v>
       </c>
       <c r="L133" s="4" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -7805,10 +7805,10 @@
         <v>37</v>
       </c>
       <c r="L134" s="6" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -7843,10 +7843,10 @@
         <v>37</v>
       </c>
       <c r="L135" s="6" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -7881,10 +7881,10 @@
         <v>37</v>
       </c>
       <c r="L136" s="10" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -7917,10 +7917,10 @@
         <v>37</v>
       </c>
       <c r="L137" s="10" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="L138" s="6"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -7991,10 +7991,10 @@
         <v>37</v>
       </c>
       <c r="L139" s="10" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -8029,10 +8029,10 @@
         <v>37</v>
       </c>
       <c r="L140" s="10" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -8067,10 +8067,10 @@
         <v>37</v>
       </c>
       <c r="L141" s="10" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -8105,10 +8105,10 @@
         <v>37</v>
       </c>
       <c r="L142" s="10" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -8143,10 +8143,10 @@
         <v>37</v>
       </c>
       <c r="L143" s="10" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -8181,10 +8181,10 @@
         <v>37</v>
       </c>
       <c r="L144" s="10" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -8219,10 +8219,10 @@
         <v>37</v>
       </c>
       <c r="L145" s="10" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -8257,10 +8257,10 @@
         <v>37</v>
       </c>
       <c r="L146" s="6" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -8295,10 +8295,10 @@
         <v>37</v>
       </c>
       <c r="L147" s="6" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -8369,10 +8369,10 @@
         <v>37</v>
       </c>
       <c r="L149" s="6" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -8407,10 +8407,10 @@
         <v>37</v>
       </c>
       <c r="L150" s="6" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -8445,10 +8445,10 @@
         <v>37</v>
       </c>
       <c r="L151" s="6" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="L152" s="4"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -8520,7 +8520,7 @@
       </c>
       <c r="L153" s="10"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -8556,7 +8556,7 @@
       </c>
       <c r="L154" s="6"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -8590,7 +8590,7 @@
       </c>
       <c r="L155" s="4"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -8624,7 +8624,7 @@
       </c>
       <c r="L156" s="4"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -8658,7 +8658,7 @@
       </c>
       <c r="L157" s="4"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -8692,7 +8692,7 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -8728,7 +8728,7 @@
       </c>
       <c r="L159" s="4"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -8764,7 +8764,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -8800,7 +8800,7 @@
       </c>
       <c r="L161" s="4"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -8836,7 +8836,7 @@
       </c>
       <c r="L162" s="10"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -8872,7 +8872,7 @@
       </c>
       <c r="L163" s="10"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -8908,7 +8908,7 @@
       </c>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="L165" s="4"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -8979,10 +8979,10 @@
         <v>8</v>
       </c>
       <c r="L166" s="10" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -9017,10 +9017,10 @@
         <v>8</v>
       </c>
       <c r="L167" s="10" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -9055,10 +9055,10 @@
         <v>8</v>
       </c>
       <c r="L168" s="10" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -9093,10 +9093,10 @@
         <v>8</v>
       </c>
       <c r="L169" s="10" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -9132,7 +9132,7 @@
       </c>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -9168,7 +9168,7 @@
       </c>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -9204,7 +9204,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -9240,7 +9240,7 @@
       </c>
       <c r="L173" s="6"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -9276,7 +9276,7 @@
       </c>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -9348,7 +9348,7 @@
       </c>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -9384,7 +9384,7 @@
       </c>
       <c r="L177" s="6"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -9420,7 +9420,7 @@
       </c>
       <c r="L178" s="6"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -9456,7 +9456,7 @@
       </c>
       <c r="L179" s="6"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="L180" s="6"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="L181" s="6"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>181</v>
       </c>
@@ -9564,7 +9564,7 @@
       </c>
       <c r="L182" s="6"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -9600,7 +9600,7 @@
       </c>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>184</v>
       </c>
@@ -9676,7 +9676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>185</v>
       </c>
@@ -9710,7 +9710,7 @@
       </c>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -9742,7 +9742,7 @@
       </c>
       <c r="L187" s="6"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -9778,7 +9778,7 @@
       </c>
       <c r="L188" s="6"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>188</v>
       </c>
@@ -9814,7 +9814,7 @@
       </c>
       <c r="L189" s="6"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>189</v>
       </c>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="L190" s="10"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>190</v>
       </c>
@@ -9882,7 +9882,7 @@
       </c>
       <c r="L191" s="10"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>191</v>
       </c>
@@ -9916,7 +9916,7 @@
       </c>
       <c r="L192" s="10"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>192</v>
       </c>
@@ -9952,7 +9952,7 @@
       </c>
       <c r="L193" s="6"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>193</v>
       </c>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="L194" s="10"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>194</v>
       </c>
@@ -10020,7 +10020,7 @@
       </c>
       <c r="L195" s="10"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>195</v>
       </c>
@@ -10054,7 +10054,7 @@
       </c>
       <c r="L196" s="10"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>196</v>
       </c>
@@ -10088,7 +10088,7 @@
       </c>
       <c r="L197" s="10"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>197</v>
       </c>
@@ -10122,7 +10122,7 @@
       </c>
       <c r="L198" s="10"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>198</v>
       </c>
@@ -10156,7 +10156,7 @@
       </c>
       <c r="L199" s="10"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>199</v>
       </c>
@@ -10190,7 +10190,7 @@
       </c>
       <c r="L200" s="10"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>200</v>
       </c>
@@ -10224,7 +10224,7 @@
       </c>
       <c r="L201" s="10"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>201</v>
       </c>
@@ -10258,7 +10258,7 @@
       </c>
       <c r="L202" s="10"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>202</v>
       </c>
@@ -10293,10 +10293,10 @@
         <v>37</v>
       </c>
       <c r="L203" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>203</v>
       </c>
@@ -10331,10 +10331,10 @@
         <v>37</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>204</v>
       </c>
@@ -10369,10 +10369,10 @@
         <v>37</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>205</v>
       </c>
@@ -10407,10 +10407,10 @@
         <v>37</v>
       </c>
       <c r="L206" s="4" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>206</v>
       </c>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>207</v>
       </c>
@@ -10481,10 +10481,10 @@
         <v>37</v>
       </c>
       <c r="L208" s="4" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>208</v>
       </c>
@@ -10520,7 +10520,7 @@
       </c>
       <c r="L209" s="4"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>209</v>
       </c>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>210</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>211</v>
       </c>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>212</v>
       </c>
@@ -10664,7 +10664,7 @@
       </c>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>213</v>
       </c>
@@ -10700,7 +10700,7 @@
       </c>
       <c r="L214" s="4"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>214</v>
       </c>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="L215" s="4"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>215</v>
       </c>
@@ -10772,7 +10772,7 @@
       </c>
       <c r="L216" s="4"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>216</v>
       </c>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="L217" s="4"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>217</v>
       </c>
@@ -10844,7 +10844,7 @@
       </c>
       <c r="L218" s="6"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>218</v>
       </c>
@@ -10880,7 +10880,7 @@
       </c>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>219</v>
       </c>
@@ -10916,7 +10916,7 @@
       </c>
       <c r="L220" s="4"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>220</v>
       </c>
@@ -10952,7 +10952,7 @@
       </c>
       <c r="L221" s="4"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>221</v>
       </c>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="L222" s="4"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>222</v>
       </c>
@@ -11021,10 +11021,10 @@
         <v>37</v>
       </c>
       <c r="L223" s="10" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>223</v>
       </c>
@@ -11059,10 +11059,10 @@
         <v>37</v>
       </c>
       <c r="L224" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>224</v>
       </c>
@@ -11095,10 +11095,10 @@
         <v>37</v>
       </c>
       <c r="L225" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>225</v>
       </c>
@@ -11131,10 +11131,10 @@
         <v>37</v>
       </c>
       <c r="L226" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>226</v>
       </c>
@@ -11167,10 +11167,10 @@
         <v>37</v>
       </c>
       <c r="L227" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="228" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>227</v>
       </c>
@@ -11203,10 +11203,10 @@
         <v>37</v>
       </c>
       <c r="L228" s="10" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>228</v>
       </c>
@@ -11239,10 +11239,10 @@
         <v>37</v>
       </c>
       <c r="L229" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>229</v>
       </c>
@@ -11275,10 +11275,10 @@
         <v>37</v>
       </c>
       <c r="L230" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>230</v>
       </c>
@@ -11311,10 +11311,10 @@
         <v>37</v>
       </c>
       <c r="L231" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="232" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>231</v>
       </c>
@@ -11347,10 +11347,10 @@
         <v>37</v>
       </c>
       <c r="L232" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>232</v>
       </c>
@@ -11383,10 +11383,10 @@
         <v>37</v>
       </c>
       <c r="L233" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>233</v>
       </c>
@@ -11419,10 +11419,10 @@
         <v>37</v>
       </c>
       <c r="L234" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>234</v>
       </c>
@@ -11455,10 +11455,10 @@
         <v>37</v>
       </c>
       <c r="L235" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>235</v>
       </c>
@@ -11493,10 +11493,10 @@
         <v>37</v>
       </c>
       <c r="L236" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>236</v>
       </c>
@@ -11529,10 +11529,10 @@
         <v>37</v>
       </c>
       <c r="L237" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>237</v>
       </c>
@@ -11567,10 +11567,10 @@
         <v>37</v>
       </c>
       <c r="L238" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>238</v>
       </c>
@@ -11603,10 +11603,10 @@
         <v>37</v>
       </c>
       <c r="L239" s="10" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="240" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>239</v>
       </c>
@@ -11641,10 +11641,10 @@
         <v>37</v>
       </c>
       <c r="L240" s="6" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="241" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>240</v>
       </c>
@@ -11679,10 +11679,10 @@
         <v>37</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="242" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>241</v>
       </c>
@@ -11717,10 +11717,10 @@
         <v>37</v>
       </c>
       <c r="L242" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="243" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>242</v>
       </c>
@@ -11755,10 +11755,10 @@
         <v>37</v>
       </c>
       <c r="L243" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="244" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>243</v>
       </c>
@@ -11793,10 +11793,10 @@
         <v>37</v>
       </c>
       <c r="L244" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="245" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>244</v>
       </c>
@@ -11831,10 +11831,10 @@
         <v>37</v>
       </c>
       <c r="L245" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="246" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>245</v>
       </c>
@@ -11869,10 +11869,10 @@
         <v>37</v>
       </c>
       <c r="L246" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="247" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>246</v>
       </c>
@@ -11907,10 +11907,10 @@
         <v>37</v>
       </c>
       <c r="L247" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="248" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>247</v>
       </c>
@@ -11945,10 +11945,10 @@
         <v>37</v>
       </c>
       <c r="L248" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="249" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>248</v>
       </c>
@@ -11983,10 +11983,10 @@
         <v>37</v>
       </c>
       <c r="L249" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="250" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>249</v>
       </c>
@@ -12021,10 +12021,10 @@
         <v>37</v>
       </c>
       <c r="L250" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="251" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>250</v>
       </c>
@@ -12059,10 +12059,10 @@
         <v>37</v>
       </c>
       <c r="L251" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="252" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>251</v>
       </c>
@@ -12097,10 +12097,10 @@
         <v>37</v>
       </c>
       <c r="L252" s="6" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>252</v>
       </c>
@@ -12136,7 +12136,7 @@
       </c>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>253</v>
       </c>
@@ -12172,7 +12172,7 @@
       </c>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>254</v>
       </c>
@@ -12208,7 +12208,7 @@
       </c>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>255</v>
       </c>
@@ -12244,7 +12244,7 @@
       </c>
       <c r="L256" s="10"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>256</v>
       </c>
@@ -12280,7 +12280,7 @@
       </c>
       <c r="L257" s="4"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>257</v>
       </c>
@@ -12316,7 +12316,7 @@
       </c>
       <c r="L258" s="6"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>258</v>
       </c>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="L259" s="4"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>259</v>
       </c>
@@ -12387,10 +12387,10 @@
         <v>8</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>260</v>
       </c>
@@ -12425,10 +12425,10 @@
         <v>8</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>261</v>
       </c>
@@ -12463,10 +12463,10 @@
         <v>8</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>262</v>
       </c>
@@ -12504,7 +12504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>263</v>
       </c>
@@ -12540,7 +12540,7 @@
       </c>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>264</v>
       </c>
@@ -12576,7 +12576,7 @@
       </c>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>265</v>
       </c>
@@ -12612,7 +12612,7 @@
       </c>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>266</v>
       </c>
@@ -12648,7 +12648,7 @@
       </c>
       <c r="L267" s="6"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>267</v>
       </c>
@@ -12682,7 +12682,7 @@
       </c>
       <c r="L268" s="10"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>268</v>
       </c>
@@ -12718,7 +12718,7 @@
       </c>
       <c r="L269" s="6"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>269</v>
       </c>
@@ -12751,10 +12751,10 @@
         <v>37</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>270</v>
       </c>
@@ -12790,7 +12790,7 @@
       </c>
       <c r="L271" s="4"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>271</v>
       </c>
@@ -12826,7 +12826,7 @@
       </c>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>272</v>
       </c>
@@ -12862,7 +12862,7 @@
       </c>
       <c r="L273" s="4"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>273</v>
       </c>
@@ -12898,7 +12898,7 @@
       </c>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>274</v>
       </c>
@@ -12934,7 +12934,7 @@
       </c>
       <c r="L275" s="6"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>275</v>
       </c>
@@ -12966,7 +12966,7 @@
       </c>
       <c r="L276" s="6"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>276</v>
       </c>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="L277" s="6"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>277</v>
       </c>
@@ -13034,7 +13034,7 @@
       </c>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>278</v>
       </c>
@@ -13070,7 +13070,7 @@
       </c>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>279</v>
       </c>
@@ -13106,7 +13106,7 @@
       </c>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>280</v>
       </c>
@@ -13142,7 +13142,7 @@
       </c>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>281</v>
       </c>
@@ -13178,7 +13178,7 @@
       </c>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A283" s="4">
         <v>282</v>
       </c>
@@ -13214,7 +13214,7 @@
       </c>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A284" s="4">
         <v>283</v>
       </c>
@@ -13249,10 +13249,10 @@
         <v>37</v>
       </c>
       <c r="L284" s="6" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A285" s="4">
         <v>284</v>
       </c>
@@ -13288,7 +13288,7 @@
       </c>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A286" s="4">
         <v>285</v>
       </c>
@@ -13323,10 +13323,10 @@
         <v>37</v>
       </c>
       <c r="L286" s="6" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A287" s="4">
         <v>286</v>
       </c>
@@ -13362,7 +13362,7 @@
       </c>
       <c r="L287" s="6"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A288" s="4">
         <v>287</v>
       </c>
@@ -13395,10 +13395,10 @@
         <v>37</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A289" s="4">
         <v>288</v>
       </c>
@@ -13431,10 +13431,10 @@
         <v>37</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="290" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A290" s="4">
         <v>289</v>
       </c>
@@ -13467,10 +13467,10 @@
         <v>37</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A291" s="4">
         <v>290</v>
       </c>
@@ -13506,7 +13506,7 @@
       </c>
       <c r="L291" s="10"/>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A292" s="4">
         <v>291</v>
       </c>
@@ -13539,10 +13539,10 @@
         <v>8</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A293" s="4">
         <v>292</v>
       </c>
@@ -13575,10 +13575,10 @@
         <v>8</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A294" s="4">
         <v>293</v>
       </c>
@@ -13614,7 +13614,7 @@
       </c>
       <c r="L294" s="4"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A295" s="4">
         <v>294</v>
       </c>
@@ -13650,7 +13650,7 @@
       </c>
       <c r="L295" s="4"/>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A296" s="4">
         <v>295</v>
       </c>
@@ -13686,7 +13686,7 @@
       </c>
       <c r="L296" s="4"/>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A297" s="4">
         <v>296</v>
       </c>
@@ -13722,7 +13722,7 @@
       </c>
       <c r="L297" s="4"/>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A298" s="4">
         <v>297</v>
       </c>
@@ -13755,10 +13755,10 @@
         <v>37</v>
       </c>
       <c r="L298" s="10" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A299" s="4">
         <v>298</v>
       </c>
@@ -13793,10 +13793,10 @@
         <v>37</v>
       </c>
       <c r="L299" s="10" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A300" s="4">
         <v>299</v>
       </c>
@@ -13829,10 +13829,10 @@
         <v>37</v>
       </c>
       <c r="L300" s="10" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A301" s="4">
         <v>300</v>
       </c>
@@ -13865,10 +13865,10 @@
         <v>37</v>
       </c>
       <c r="L301" s="10" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A302" s="4">
         <v>301</v>
       </c>
@@ -13903,10 +13903,10 @@
         <v>37</v>
       </c>
       <c r="L302" s="4" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A303" s="4">
         <v>302</v>
       </c>
@@ -13941,10 +13941,10 @@
         <v>37</v>
       </c>
       <c r="L303" s="4" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A304" s="4">
         <v>303</v>
       </c>
@@ -13979,10 +13979,10 @@
         <v>37</v>
       </c>
       <c r="L304" s="4" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A305" s="4">
         <v>304</v>
       </c>
@@ -14017,10 +14017,10 @@
         <v>37</v>
       </c>
       <c r="L305" s="10" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A306" s="4">
         <v>305</v>
       </c>
@@ -14054,7 +14054,7 @@
       </c>
       <c r="L306" s="6"/>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A307" s="4">
         <v>306</v>
       </c>
@@ -14089,10 +14089,10 @@
         <v>37</v>
       </c>
       <c r="L307" s="6" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A308" s="4">
         <v>307</v>
       </c>
@@ -14127,10 +14127,10 @@
         <v>37</v>
       </c>
       <c r="L308" s="6" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A309" s="4">
         <v>308</v>
       </c>
@@ -14165,10 +14165,10 @@
         <v>37</v>
       </c>
       <c r="L309" s="4" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A310" s="4">
         <v>309</v>
       </c>
@@ -14204,7 +14204,7 @@
       </c>
       <c r="L310" s="4"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A311" s="4">
         <v>310</v>
       </c>
@@ -14240,7 +14240,7 @@
       </c>
       <c r="L311" s="4"/>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A312" s="4">
         <v>311</v>
       </c>
@@ -14276,7 +14276,7 @@
       </c>
       <c r="L312" s="4"/>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A313" s="4">
         <v>312</v>
       </c>
@@ -14312,7 +14312,7 @@
       </c>
       <c r="L313" s="4"/>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A314" s="4">
         <v>313</v>
       </c>
@@ -14348,7 +14348,7 @@
       </c>
       <c r="L314" s="6"/>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A315" s="4">
         <v>314</v>
       </c>
@@ -14384,7 +14384,7 @@
       </c>
       <c r="L315" s="6"/>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A316" s="4">
         <v>315</v>
       </c>
@@ -14420,7 +14420,7 @@
       </c>
       <c r="L316" s="6"/>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A317" s="4">
         <v>316</v>
       </c>
@@ -14455,10 +14455,10 @@
         <v>37</v>
       </c>
       <c r="L317" s="4" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="318" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A318" s="4">
         <v>317</v>
       </c>
@@ -14493,10 +14493,10 @@
         <v>37</v>
       </c>
       <c r="L318" s="6" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="319" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A319" s="4">
         <v>318</v>
       </c>
@@ -14531,10 +14531,10 @@
         <v>37</v>
       </c>
       <c r="L319" s="6" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="320" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A320" s="4">
         <v>319</v>
       </c>
@@ -14569,10 +14569,10 @@
         <v>37</v>
       </c>
       <c r="L320" s="6" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="321" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A321" s="4">
         <v>320</v>
       </c>
@@ -14607,10 +14607,10 @@
         <v>37</v>
       </c>
       <c r="L321" s="6" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="322" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A322" s="4">
         <v>321</v>
       </c>
@@ -14645,10 +14645,10 @@
         <v>37</v>
       </c>
       <c r="L322" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A323" s="4">
         <v>322</v>
       </c>
@@ -14683,10 +14683,10 @@
         <v>37</v>
       </c>
       <c r="L323" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A324" s="4">
         <v>323</v>
       </c>
@@ -14721,10 +14721,10 @@
         <v>37</v>
       </c>
       <c r="L324" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A325" s="4">
         <v>324</v>
       </c>
@@ -14759,10 +14759,10 @@
         <v>37</v>
       </c>
       <c r="L325" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A326" s="4">
         <v>325</v>
       </c>
@@ -14797,10 +14797,10 @@
         <v>37</v>
       </c>
       <c r="L326" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A327" s="4">
         <v>326</v>
       </c>
@@ -14835,10 +14835,10 @@
         <v>37</v>
       </c>
       <c r="L327" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A328" s="4">
         <v>327</v>
       </c>
@@ -14873,10 +14873,10 @@
         <v>37</v>
       </c>
       <c r="L328" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="329" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A329" s="4">
         <v>328</v>
       </c>
@@ -14911,10 +14911,10 @@
         <v>37</v>
       </c>
       <c r="L329" s="6" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="330" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A330" s="4">
         <v>329</v>
       </c>
@@ -14949,10 +14949,10 @@
         <v>37</v>
       </c>
       <c r="L330" s="6" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A331" s="4">
         <v>330</v>
       </c>
@@ -14988,7 +14988,7 @@
       </c>
       <c r="L331" s="6"/>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A332" s="4">
         <v>331</v>
       </c>

</xml_diff>